<commit_message>
made functions and before cleaning up
</commit_message>
<xml_diff>
--- a/_class_tt.xlsx
+++ b/_class_tt.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365"/>
   </bookViews>
   <sheets>
-    <sheet name="Faculty _TT " sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="__xlnm.Print_Area" localSheetId="0">'Faculty _TT '!$A$1:$L$15</definedName>
+    <definedName name="__xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$L$15</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <extLst>
@@ -620,6 +620,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -649,12 +655,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -710,10 +710,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1012,7 +1012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z979"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1035,7 +1037,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="17"/>
-      <c r="B1" s="44"/>
+      <c r="B1" s="46"/>
       <c r="C1" s="9">
         <v>1</v>
       </c>
@@ -1053,8 +1055,8 @@
       <c r="I1" s="22">
         <v>5</v>
       </c>
-      <c r="J1" s="69"/>
-      <c r="K1" s="68">
+      <c r="J1" s="39"/>
+      <c r="K1" s="38">
         <v>6</v>
       </c>
       <c r="L1" s="22">
@@ -1079,7 +1081,7 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A2" s="18"/>
-      <c r="B2" s="45"/>
+      <c r="B2" s="47"/>
       <c r="C2" s="29" t="s">
         <v>9</v>
       </c>
@@ -1099,7 +1101,7 @@
       <c r="I2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="69"/>
+      <c r="J2" s="39"/>
       <c r="K2" s="13" t="s">
         <v>2</v>
       </c>
@@ -1122,10 +1124,10 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="25" t="s">
@@ -1164,8 +1166,8 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="39"/>
-      <c r="B4" s="43"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="25"/>
       <c r="D4" s="24"/>
       <c r="E4" s="56"/>
@@ -1192,8 +1194,8 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A5" s="39"/>
-      <c r="B5" s="42" t="s">
+      <c r="A5" s="41"/>
+      <c r="B5" s="44" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="23" t="s">
@@ -1232,8 +1234,8 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A6" s="39"/>
-      <c r="B6" s="43"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="30" t="s">
         <v>16</v>
       </c>
@@ -1262,8 +1264,8 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A7" s="39"/>
-      <c r="B7" s="42" t="s">
+      <c r="A7" s="41"/>
+      <c r="B7" s="44" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -1298,8 +1300,8 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A8" s="39"/>
-      <c r="B8" s="43"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="25"/>
       <c r="D8" s="62" t="s">
         <v>13</v>
@@ -1328,8 +1330,8 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A9" s="39"/>
-      <c r="B9" s="42" t="s">
+      <c r="A9" s="41"/>
+      <c r="B9" s="44" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="31" t="s">
@@ -1368,7 +1370,7 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A10" s="39"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="63"/>
       <c r="C10" s="32" t="s">
         <v>16</v>
@@ -1378,7 +1380,7 @@
       <c r="F10" s="33"/>
       <c r="G10" s="34"/>
       <c r="H10" s="66"/>
-      <c r="I10" s="48"/>
+      <c r="I10" s="68"/>
       <c r="J10" s="62"/>
       <c r="K10" s="62"/>
       <c r="L10" s="62"/>
@@ -1398,8 +1400,8 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" s="21" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A11" s="40"/>
-      <c r="B11" s="46" t="s">
+      <c r="A11" s="42"/>
+      <c r="B11" s="48" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="29" t="s">
@@ -1442,8 +1444,8 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A12" s="40"/>
-      <c r="B12" s="47"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="28" t="s">
         <v>21</v>
       </c>
@@ -1479,8 +1481,8 @@
       <c r="Y12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A13" s="40"/>
-      <c r="B13" s="47"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
       <c r="E13" s="60"/>
@@ -1489,10 +1491,10 @@
       </c>
       <c r="G13" s="34"/>
       <c r="H13" s="65"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="49"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="69"/>
       <c r="M13" s="67"/>
       <c r="N13" s="67"/>
       <c r="O13" s="1"/>
@@ -1508,7 +1510,7 @@
       <c r="Y13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A14" s="40"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="50" t="s">
         <v>14</v>
       </c>
@@ -1540,7 +1542,7 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A15" s="41"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="51"/>
       <c r="C15" s="53"/>
       <c r="D15" s="53"/>
@@ -23267,7 +23269,6 @@
     <mergeCell ref="I9:L9"/>
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I13:L13"/>
-    <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:L15"/>
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="E9:E13"/>
@@ -23284,6 +23285,7 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0.43333333333333335" right="0.2" top="0.2298611111111111" bottom="0.3298611111111111" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>